<commit_message>
Generar variables faltantes para el armado de los proceso  (rutas y nombre de archivo)
Procedimiento de armado de ruta de los archivos (generacion ambiente de de prueba ) “\reportes\web_reports\ BOSCH”, “\reportes\web_reports\ GSK”,
Ajustar el proceso para integrar los ajustes nuevos del punto 1 (procedimienti, creación de parametros)
Se ajustó el proceso de GSK (el reporte no  toma ningún parámetro, se ajustó para tomar el parametro_1 de la tabla de reporte_detalle )
Se genero la publicación de la aplicación, la cual recibe como parámetro el id_cron  y el tipo
Ruta de publicación 01-CodigoFuente\main\Spooler\main\main\public \reportes
</commit_message>
<xml_diff>
--- a/01-CodigoFuente/main/Spooler/main/main/bin/Debug/net8.0/spread_Transmision_EDOCs_18975_may-01-2024may-31-2024.xlsx
+++ b/01-CodigoFuente/main/Spooler/main/main/bin/Debug/net8.0/spread_Transmision_EDOCs_18975_may-01-2024may-31-2024.xlsx
@@ -6,8 +6,8 @@
     <x:workbookView activeTab="1"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Exportación" sheetId="1" r:id="R42641094c22f4100"/>
-    <x:sheet name="Importación" sheetId="2" r:id="Re3d2ac5543714fa4"/>
+    <x:sheet name="Exportación" sheetId="1" r:id="R5a415b183447491c"/>
+    <x:sheet name="Importación" sheetId="2" r:id="Rfef700b9e5be4883"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>